<commit_message>
updated tufts mapping to include S17
</commit_message>
<xml_diff>
--- a/_site/projects/nhl-projections/files/data/projection_output.xlsx
+++ b/_site/projects/nhl-projections/files/data/projection_output.xlsx
@@ -528,7 +528,7 @@
         <v>2</v>
       </c>
       <c r="D2" s="4">
-        <v>42662</v>
+        <v>42787</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -777,7 +777,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -809,15 +809,15 @@
       </c>
       <c r="B2" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A2,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A2,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>4.32</v>
+        <v>66.930000000000007</v>
       </c>
       <c r="D2" s="1" t="str">
         <f>IFERROR(IF(C2&gt;B2,"+","-")&amp;ROUND(ABS(C2-B2),2),"-")</f>
-        <v>+3.32</v>
+        <v>+66.93</v>
       </c>
       <c r="E2" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!$B:$B)-1,MATCH(output!$A2,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -835,15 +835,15 @@
       </c>
       <c r="B3" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A3,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A3,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>1.67</v>
+        <v>60.28</v>
       </c>
       <c r="D3" s="1" t="str">
         <f t="shared" ref="D3:D7" si="0">IFERROR(IF(C3&gt;B3,"+","-")&amp;ROUND(ABS(C3-B3),2),"-")</f>
-        <v>-0.33</v>
+        <v>+60.28</v>
       </c>
       <c r="E3" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A3,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -861,15 +861,15 @@
       </c>
       <c r="B4" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A4,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A4,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>3.78</v>
+        <v>66.400000000000006</v>
       </c>
       <c r="D4" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>-0.22</v>
+        <v>+66.4</v>
       </c>
       <c r="E4" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A4,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -887,15 +887,15 @@
       </c>
       <c r="B5" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A5,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A5,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>3.41</v>
+        <v>58.42</v>
       </c>
       <c r="D5" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>+0.41</v>
+        <v>+58.42</v>
       </c>
       <c r="E5" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A5,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -913,15 +913,15 @@
       </c>
       <c r="B6" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A6,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A6,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>4.58</v>
+        <v>62.04</v>
       </c>
       <c r="D6" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>+1.58</v>
+        <v>+62.04</v>
       </c>
       <c r="E6" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A6,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -939,15 +939,15 @@
       </c>
       <c r="B7" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A7,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C7" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A7,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>2.92</v>
+        <v>52.22</v>
       </c>
       <c r="D7" s="1" t="str">
         <f t="shared" si="0"/>
-        <v>+0.92</v>
+        <v>+52.22</v>
       </c>
       <c r="E7" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A7,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -965,15 +965,15 @@
       </c>
       <c r="B8" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A8,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C8" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A8,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>4.12</v>
+        <v>68.38</v>
       </c>
       <c r="D8" s="1" t="str">
         <f t="shared" ref="D8:D31" si="1">IFERROR(IF(C8&gt;B8,"+","-")&amp;ROUND(ABS(C8-B8),2),"-")</f>
-        <v>+0.12</v>
+        <v>+68.38</v>
       </c>
       <c r="E8" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A8,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -991,15 +991,15 @@
       </c>
       <c r="B9" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A9,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C9" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A9,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>3.18</v>
+        <v>61.92</v>
       </c>
       <c r="D9" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>-0.82</v>
+        <v>+61.92</v>
       </c>
       <c r="E9" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A9,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1021,11 +1021,11 @@
       </c>
       <c r="C10" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A10,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>1.71</v>
+        <v>55.37</v>
       </c>
       <c r="D10" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>+1.71</v>
+        <v>+55.37</v>
       </c>
       <c r="E10" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A10,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1043,15 +1043,15 @@
       </c>
       <c r="B11" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A11,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C11" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A11,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>3.35</v>
+        <v>70.88</v>
       </c>
       <c r="D11" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>-0.65</v>
+        <v>+70.88</v>
       </c>
       <c r="E11" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A11,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1069,15 +1069,15 @@
       </c>
       <c r="B12" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A12,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C12" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A12,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>2.96</v>
+        <v>63.02</v>
       </c>
       <c r="D12" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>-1.04</v>
+        <v>+63.02</v>
       </c>
       <c r="E12" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A12,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1095,15 +1095,15 @@
       </c>
       <c r="B13" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A13,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C13" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A13,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>3.98</v>
+        <v>57.41</v>
       </c>
       <c r="D13" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>-2.02</v>
+        <v>+57.41</v>
       </c>
       <c r="E13" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A13,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1121,15 +1121,15 @@
       </c>
       <c r="B14" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A14,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C14" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A14,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>3.21</v>
+        <v>62.57</v>
       </c>
       <c r="D14" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>-1.79</v>
+        <v>+62.57</v>
       </c>
       <c r="E14" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A14,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1151,11 +1151,11 @@
       </c>
       <c r="C15" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A15,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>2.96</v>
+        <v>61.34</v>
       </c>
       <c r="D15" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>+2.96</v>
+        <v>+61.34</v>
       </c>
       <c r="E15" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A15,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1173,15 +1173,15 @@
       </c>
       <c r="B16" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A16,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C16" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A16,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>3.06</v>
+        <v>61.76</v>
       </c>
       <c r="D16" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>-0.94</v>
+        <v>+61.76</v>
       </c>
       <c r="E16" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A16,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1199,15 +1199,15 @@
       </c>
       <c r="B17" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A17,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C17" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A17,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>3.13</v>
+        <v>61.4</v>
       </c>
       <c r="D17" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>-1.87</v>
+        <v>+61.4</v>
       </c>
       <c r="E17" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A17,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1225,15 +1225,15 @@
       </c>
       <c r="B18" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A18,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C18" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A18,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>2.94</v>
+        <v>61.62</v>
       </c>
       <c r="D18" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>+0.94</v>
+        <v>+61.62</v>
       </c>
       <c r="E18" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A18,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1251,15 +1251,15 @@
       </c>
       <c r="B19" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A19,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C19" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A19,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>2.8</v>
+        <v>58.63</v>
       </c>
       <c r="D19" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>-0.2</v>
+        <v>+58.63</v>
       </c>
       <c r="E19" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A19,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1277,15 +1277,15 @@
       </c>
       <c r="B20" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A20,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C20" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A20,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>3.92</v>
+        <v>60.89</v>
       </c>
       <c r="D20" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>+1.92</v>
+        <v>+60.89</v>
       </c>
       <c r="E20" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A20,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1303,15 +1303,15 @@
       </c>
       <c r="B21" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A21,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C21" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A21,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>3.43</v>
+        <v>66.7</v>
       </c>
       <c r="D21" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>-0.57</v>
+        <v>+66.7</v>
       </c>
       <c r="E21" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A21,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1329,15 +1329,15 @@
       </c>
       <c r="B22" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A22,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C22" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A22,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>4.37</v>
+        <v>63.81</v>
       </c>
       <c r="D22" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>-1.63</v>
+        <v>+63.81</v>
       </c>
       <c r="E22" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A22,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1355,15 +1355,15 @@
       </c>
       <c r="B23" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A23,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C23" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A23,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>3.66</v>
+        <v>63.61</v>
       </c>
       <c r="D23" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>+0.66</v>
+        <v>+63.61</v>
       </c>
       <c r="E23" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A23,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1381,15 +1381,15 @@
       </c>
       <c r="B24" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A24,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C24" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A24,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>4.68</v>
+        <v>67.400000000000006</v>
       </c>
       <c r="D24" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>-0.32</v>
+        <v>+67.4</v>
       </c>
       <c r="E24" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A24,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1407,15 +1407,15 @@
       </c>
       <c r="B25" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A25,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C25" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A25,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>4.4000000000000004</v>
+        <v>68.150000000000006</v>
       </c>
       <c r="D25" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>-1.6</v>
+        <v>+68.15</v>
       </c>
       <c r="E25" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A25,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1433,15 +1433,15 @@
       </c>
       <c r="B26" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A26,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="C26" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A26,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>4.78</v>
+        <v>67.459999999999994</v>
       </c>
       <c r="D26" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>-2.22</v>
+        <v>+67.46</v>
       </c>
       <c r="E26" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A26,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1459,15 +1459,15 @@
       </c>
       <c r="B27" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A27,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C27" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A27,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>3.54</v>
+        <v>65.959999999999994</v>
       </c>
       <c r="D27" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>-2.46</v>
+        <v>+65.96</v>
       </c>
       <c r="E27" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A27,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1485,15 +1485,15 @@
       </c>
       <c r="B28" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A28,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C28" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A28,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>1.89</v>
+        <v>57.78</v>
       </c>
       <c r="D28" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>-2.11</v>
+        <v>+57.78</v>
       </c>
       <c r="E28" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A28,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1511,15 +1511,15 @@
       </c>
       <c r="B29" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A29,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="C29" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A29,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>2.82</v>
+        <v>55.37</v>
       </c>
       <c r="D29" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>-3.18</v>
+        <v>+55.37</v>
       </c>
       <c r="E29" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A29,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1537,15 +1537,15 @@
       </c>
       <c r="B30" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A30,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="C30" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A30,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>3</v>
+        <v>63.4</v>
       </c>
       <c r="D30" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>-2</v>
+        <v>+63.4</v>
       </c>
       <c r="E30" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A30,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1563,15 +1563,15 @@
       </c>
       <c r="B31" s="1">
         <f>IFERROR(INDEX('raw actual'!$A$1:$AF$367,MATCH(variables!$D$2,'raw actual'!$A$1:$A$367,0),MATCH($A31,'raw actual'!$A$1:$AF$1,0)),"-")</f>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="C31" s="1">
         <f>IFERROR(INDEX('raw curr proj'!$A$1:$AF$367,MATCH(variables!$D$2,'raw curr proj'!$A$1:$A$367,0),MATCH($A31,'raw curr proj'!$A$1:$AF$1,0)),"-")</f>
-        <v>3.24</v>
+        <v>62.66</v>
       </c>
       <c r="D31" s="1" t="str">
         <f t="shared" si="1"/>
-        <v>-0.76</v>
+        <v>+62.66</v>
       </c>
       <c r="E31" s="1">
         <f ca="1">OFFSET('raw curr proj'!$B$1,COUNTA('raw curr proj'!B:B)-1,MATCH(output!A31,'raw curr proj'!$C$1:$AF$1,0))</f>
@@ -1595,7 +1595,7 @@
   <dimension ref="A1:AE367"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B191" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B343" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
       <selection pane="bottomRight" activeCell="AF202" sqref="AF202"/>

</xml_diff>